<commit_message>
portal page added, php modifications yet
</commit_message>
<xml_diff>
--- a/portal/pages/functions/uploads/AdminLTE 3  DataTables.xlsx
+++ b/portal/pages/functions/uploads/AdminLTE 3  DataTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myPC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BFCE2F-658B-40A9-AA42-C3344E65215F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F3F7A0-06E4-487E-84B1-59FF6EC10EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>